<commit_message>
added home depot receipt
</commit_message>
<xml_diff>
--- a/reciepts/Casey/Casey Costs.xlsx
+++ b/reciepts/Casey/Casey Costs.xlsx
@@ -265,6 +265,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -273,13 +280,6 @@
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -591,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28:H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,11 +646,11 @@
       <c r="F3">
         <v>3</v>
       </c>
-      <c r="G3" s="8">
-        <f>F3*E3</f>
+      <c r="G3" s="5">
+        <f t="shared" ref="G3:G25" si="0">F3*E3</f>
         <v>86.85</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="6">
         <v>24.68</v>
       </c>
     </row>
@@ -670,11 +670,11 @@
       <c r="F4">
         <v>14</v>
       </c>
-      <c r="G4" s="8">
-        <f>F4*E4</f>
+      <c r="G4" s="5">
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="H4" s="9"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
@@ -692,11 +692,11 @@
       <c r="F5">
         <v>5</v>
       </c>
-      <c r="G5" s="8">
-        <f>F5*E5</f>
+      <c r="G5" s="5">
+        <f t="shared" si="0"/>
         <v>34.75</v>
       </c>
-      <c r="H5" s="9"/>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
@@ -714,11 +714,11 @@
       <c r="F6">
         <v>2</v>
       </c>
-      <c r="G6" s="8">
-        <f>F6*E6</f>
+      <c r="G6" s="5">
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="H6" s="9"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
@@ -736,11 +736,11 @@
       <c r="F7">
         <v>4</v>
       </c>
-      <c r="G7" s="8">
-        <f>F7*E7</f>
+      <c r="G7" s="5">
+        <f t="shared" si="0"/>
         <v>27.8</v>
       </c>
-      <c r="H7" s="9"/>
+      <c r="H7" s="6"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
@@ -758,11 +758,11 @@
       <c r="F8">
         <v>2</v>
       </c>
-      <c r="G8" s="8">
-        <f>F8*E8</f>
+      <c r="G8" s="5">
+        <f t="shared" si="0"/>
         <v>13.9</v>
       </c>
-      <c r="H8" s="9"/>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
@@ -780,11 +780,11 @@
       <c r="F9">
         <v>1</v>
       </c>
-      <c r="G9" s="8">
-        <f>F9*E9</f>
-        <v>11</v>
-      </c>
-      <c r="H9" s="9"/>
+      <c r="G9" s="5">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
@@ -802,11 +802,11 @@
       <c r="F10">
         <v>10</v>
       </c>
-      <c r="G10" s="8">
-        <f>F10*E10</f>
+      <c r="G10" s="5">
+        <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
-      <c r="H10" s="9"/>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
@@ -824,11 +824,11 @@
       <c r="F11">
         <v>8</v>
       </c>
-      <c r="G11" s="8">
-        <f>F11*E11</f>
+      <c r="G11" s="5">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="H11" s="9"/>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
@@ -846,11 +846,11 @@
       <c r="F12">
         <v>1</v>
       </c>
-      <c r="G12" s="8">
-        <f>F12*E12</f>
+      <c r="G12" s="5">
+        <f t="shared" si="0"/>
         <v>5.45</v>
       </c>
-      <c r="H12" s="9"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
@@ -868,11 +868,11 @@
       <c r="F13">
         <v>36</v>
       </c>
-      <c r="G13" s="8">
-        <f>F13*E13</f>
+      <c r="G13" s="5">
+        <f t="shared" si="0"/>
         <v>5.3999999999999995</v>
       </c>
-      <c r="H13" s="9"/>
+      <c r="H13" s="6"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
@@ -890,11 +890,11 @@
       <c r="F14">
         <v>1</v>
       </c>
-      <c r="G14" s="8">
-        <f>F14*E14</f>
+      <c r="G14" s="5">
+        <f t="shared" si="0"/>
         <v>4.95</v>
       </c>
-      <c r="H14" s="9"/>
+      <c r="H14" s="6"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
@@ -912,11 +912,11 @@
       <c r="F15">
         <v>6</v>
       </c>
-      <c r="G15" s="8">
-        <f>F15*E15</f>
+      <c r="G15" s="5">
+        <f t="shared" si="0"/>
         <v>3.5999999999999996</v>
       </c>
-      <c r="H15" s="9"/>
+      <c r="H15" s="6"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
@@ -934,11 +934,11 @@
       <c r="F16">
         <v>1</v>
       </c>
-      <c r="G16" s="8">
-        <f>F16*E16</f>
-        <v>1</v>
-      </c>
-      <c r="H16" s="9"/>
+      <c r="G16" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
@@ -956,11 +956,11 @@
       <c r="F17">
         <v>2</v>
       </c>
-      <c r="G17" s="8">
-        <f>F17*E17</f>
+      <c r="G17" s="5">
+        <f t="shared" si="0"/>
         <v>34.9</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="4">
         <v>0</v>
       </c>
     </row>
@@ -980,11 +980,11 @@
       <c r="F18">
         <v>2</v>
       </c>
-      <c r="G18" s="8">
-        <f>F18*E18</f>
+      <c r="G18" s="5">
+        <f t="shared" si="0"/>
         <v>29.98</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="6">
         <v>0</v>
       </c>
     </row>
@@ -1004,11 +1004,11 @@
       <c r="F19">
         <v>2</v>
       </c>
-      <c r="G19" s="8">
-        <f>F19*E19</f>
+      <c r="G19" s="5">
+        <f t="shared" si="0"/>
         <v>27.98</v>
       </c>
-      <c r="H19" s="9"/>
+      <c r="H19" s="6"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
@@ -1026,11 +1026,11 @@
       <c r="F20">
         <v>1</v>
       </c>
-      <c r="G20" s="8">
-        <f>F20*E20</f>
+      <c r="G20" s="5">
+        <f t="shared" si="0"/>
         <v>26.99</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H20" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1050,11 +1050,11 @@
       <c r="F21">
         <v>1</v>
       </c>
-      <c r="G21" s="8">
-        <f>F21*E21</f>
+      <c r="G21" s="5">
+        <f t="shared" si="0"/>
         <v>10.95</v>
       </c>
-      <c r="H21" s="7">
+      <c r="H21" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1074,11 +1074,11 @@
       <c r="F22">
         <v>1</v>
       </c>
-      <c r="G22" s="8">
-        <f>F22*E22</f>
+      <c r="G22" s="5">
+        <f t="shared" si="0"/>
         <v>10.78</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H22" s="6">
         <v>0</v>
       </c>
     </row>
@@ -1098,11 +1098,11 @@
       <c r="F23">
         <v>1</v>
       </c>
-      <c r="G23" s="8">
-        <f>F23*E23</f>
+      <c r="G23" s="5">
+        <f t="shared" si="0"/>
         <v>5.09</v>
       </c>
-      <c r="H23" s="9"/>
+      <c r="H23" s="6"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
@@ -1120,11 +1120,11 @@
       <c r="F24">
         <v>1</v>
       </c>
-      <c r="G24" s="8">
-        <f>F24*E24</f>
+      <c r="G24" s="5">
+        <f t="shared" si="0"/>
         <v>7.92</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H24" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1144,11 +1144,11 @@
       <c r="F25">
         <v>1</v>
       </c>
-      <c r="G25" s="8">
-        <f>F25*E25</f>
+      <c r="G25" s="5">
+        <f t="shared" si="0"/>
         <v>5.87</v>
       </c>
-      <c r="H25" s="7">
+      <c r="H25" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1163,61 +1163,61 @@
         <v>59</v>
       </c>
       <c r="E26" s="1">
-        <v>20</v>
+        <v>19.63</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
-      <c r="G26" s="8">
-        <f t="shared" ref="G26" si="0">F26*E26</f>
-        <v>20</v>
-      </c>
-      <c r="H26" s="7">
+      <c r="G26" s="5">
+        <f t="shared" ref="G26" si="1">F26*E26</f>
+        <v>19.63</v>
+      </c>
+      <c r="H26" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="5">
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="8">
         <f>SUM(G3:G26)</f>
-        <v>459.65999999999997</v>
-      </c>
-      <c r="H28" s="5"/>
+        <v>459.28999999999996</v>
+      </c>
+      <c r="H28" s="8"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="6">
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="9">
         <f>SUM(H3:H26)</f>
         <v>24.68</v>
       </c>
-      <c r="H29" s="6"/>
+      <c r="H29" s="9"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
       <c r="G30" s="10">
         <f>SUM(G28:H29)</f>
-        <v>484.34</v>
+        <v>483.96999999999997</v>
       </c>
       <c r="H30" s="10"/>
     </row>

</xml_diff>

<commit_message>
adjusted burn time per pixel.
</commit_message>
<xml_diff>
--- a/reciepts/Casey/Casey Costs.xlsx
+++ b/reciepts/Casey/Casey Costs.xlsx
@@ -663,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:F42"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1265,7 +1265,7 @@
         <v>1</v>
       </c>
       <c r="G27" s="5">
-        <f>F27*E27</f>
+        <f t="shared" ref="G27:G38" si="1">F27*E27</f>
         <v>19.63</v>
       </c>
       <c r="H27" s="4">
@@ -1289,7 +1289,7 @@
         <v>1</v>
       </c>
       <c r="G28" s="5">
-        <f>F28*E28</f>
+        <f t="shared" si="1"/>
         <v>11.04</v>
       </c>
       <c r="H28" s="4">
@@ -1313,7 +1313,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="5">
-        <f>F29*E29</f>
+        <f t="shared" si="1"/>
         <v>7.46</v>
       </c>
       <c r="H29" s="4">
@@ -1337,7 +1337,7 @@
         <v>1</v>
       </c>
       <c r="G30" s="5">
-        <f>F30*E30</f>
+        <f t="shared" si="1"/>
         <v>7.35</v>
       </c>
       <c r="H30" s="4">
@@ -1361,7 +1361,7 @@
         <v>1</v>
       </c>
       <c r="G31" s="5">
-        <f>F31*E31</f>
+        <f t="shared" si="1"/>
         <v>6.9</v>
       </c>
       <c r="H31" s="4">
@@ -1385,7 +1385,7 @@
         <v>6</v>
       </c>
       <c r="G32" s="5">
-        <f>F32*E32</f>
+        <f t="shared" si="1"/>
         <v>2.88</v>
       </c>
       <c r="H32" s="4">
@@ -1409,7 +1409,7 @@
         <v>1</v>
       </c>
       <c r="G33" s="5">
-        <f>F33*E33</f>
+        <f t="shared" si="1"/>
         <v>2.84</v>
       </c>
       <c r="H33" s="4">
@@ -1433,7 +1433,7 @@
         <v>3</v>
       </c>
       <c r="G34" s="5">
-        <f>F34*E34</f>
+        <f t="shared" si="1"/>
         <v>1.44</v>
       </c>
       <c r="H34" s="4">
@@ -1457,7 +1457,7 @@
         <v>1</v>
       </c>
       <c r="G35" s="5">
-        <f>F35*E35</f>
+        <f t="shared" si="1"/>
         <v>4.25</v>
       </c>
       <c r="H35" s="4">
@@ -1481,7 +1481,7 @@
         <v>1</v>
       </c>
       <c r="G36" s="5">
-        <f>F36*E36</f>
+        <f t="shared" si="1"/>
         <v>3.18</v>
       </c>
       <c r="H36" s="4">
@@ -1505,7 +1505,7 @@
         <v>1</v>
       </c>
       <c r="G37" s="5">
-        <f>F37*E37</f>
+        <f t="shared" si="1"/>
         <v>1.58</v>
       </c>
       <c r="H37" s="4">
@@ -1529,7 +1529,7 @@
         <v>1</v>
       </c>
       <c r="G38" s="5">
-        <f>F38*E38</f>
+        <f t="shared" si="1"/>
         <v>1.05</v>
       </c>
       <c r="H38" s="4">

</xml_diff>

<commit_message>
updated GUI slightly, receipts
</commit_message>
<xml_diff>
--- a/reciepts/Casey/Casey Costs.xlsx
+++ b/reciepts/Casey/Casey Costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="84">
   <si>
     <t>P/N</t>
   </si>
@@ -661,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H51"/>
+  <dimension ref="A2:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,7 +719,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="5">
-        <f t="shared" ref="G3:G26" si="0">F3*E3</f>
+        <f t="shared" ref="G3:G27" si="0">F3*E3</f>
         <v>86.85</v>
       </c>
       <c r="H3" s="6">
@@ -1259,14 +1259,14 @@
         <v>59</v>
       </c>
       <c r="E27" s="1">
-        <v>19.63</v>
+        <v>21.66</v>
       </c>
       <c r="F27">
         <v>1</v>
       </c>
       <c r="G27" s="5">
-        <f t="shared" ref="G27:G38" si="1">F27*E27</f>
-        <v>19.63</v>
+        <f t="shared" si="0"/>
+        <v>21.66</v>
       </c>
       <c r="H27" s="4">
         <v>0</v>
@@ -1277,315 +1277,333 @@
         <v>57</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D28" t="s">
         <v>59</v>
       </c>
       <c r="E28" s="1">
+        <v>19.63</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28" s="5">
+        <f t="shared" ref="G28:G39" si="1">F28*E28</f>
+        <v>19.63</v>
+      </c>
+      <c r="H28" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" s="1">
         <v>11.04</v>
       </c>
-      <c r="F28">
-        <v>1</v>
-      </c>
-      <c r="G28" s="5">
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29" s="5">
         <f t="shared" si="1"/>
         <v>11.04</v>
       </c>
-      <c r="H28" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="2" t="s">
+      <c r="H29" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>83</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>59</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E30" s="1">
         <v>7.46</v>
       </c>
-      <c r="F29">
-        <v>1</v>
-      </c>
-      <c r="G29" s="5">
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30" s="5">
         <f t="shared" si="1"/>
         <v>7.46</v>
       </c>
-      <c r="H29" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="2" t="s">
+      <c r="H30" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>79</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D31" t="s">
         <v>59</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E31" s="1">
         <v>7.35</v>
       </c>
-      <c r="F30">
-        <v>1</v>
-      </c>
-      <c r="G30" s="5">
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31" s="5">
         <f t="shared" si="1"/>
         <v>7.35</v>
       </c>
-      <c r="H30" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
+      <c r="H31" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>81</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D32" t="s">
         <v>59</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E32" s="1">
         <v>6.9</v>
       </c>
-      <c r="F31">
-        <v>1</v>
-      </c>
-      <c r="G31" s="5">
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32" s="5">
         <f t="shared" si="1"/>
         <v>6.9</v>
       </c>
-      <c r="H31" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="2" t="s">
+      <c r="H32" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>65</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>59</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E33" s="1">
         <v>0.48</v>
       </c>
-      <c r="F32">
+      <c r="F33">
         <v>6</v>
       </c>
-      <c r="G32" s="5">
+      <c r="G33" s="5">
         <f t="shared" si="1"/>
         <v>2.88</v>
       </c>
-      <c r="H32" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="2" t="s">
+      <c r="H33" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>67</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D34" t="s">
         <v>59</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E34" s="1">
         <v>2.84</v>
       </c>
-      <c r="F33">
-        <v>1</v>
-      </c>
-      <c r="G33" s="5">
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34" s="5">
         <f t="shared" si="1"/>
         <v>2.84</v>
       </c>
-      <c r="H33" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="2" t="s">
+      <c r="H34" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>63</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>59</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E35" s="1">
         <v>0.48</v>
       </c>
-      <c r="F34">
+      <c r="F35">
         <v>3</v>
       </c>
-      <c r="G34" s="5">
+      <c r="G35" s="5">
         <f t="shared" si="1"/>
         <v>1.44</v>
       </c>
-      <c r="H34" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="2" t="s">
+      <c r="H35" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>69</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>70</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E36" s="1">
         <v>4.25</v>
       </c>
-      <c r="F35">
-        <v>1</v>
-      </c>
-      <c r="G35" s="5">
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36" s="5">
         <f t="shared" si="1"/>
         <v>4.25</v>
       </c>
-      <c r="H35" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="2" t="s">
+      <c r="H36" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>73</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>70</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E37" s="1">
         <v>3.18</v>
       </c>
-      <c r="F36">
-        <v>1</v>
-      </c>
-      <c r="G36" s="5">
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37" s="5">
         <f t="shared" si="1"/>
         <v>3.18</v>
       </c>
-      <c r="H36" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="2" t="s">
+      <c r="H37" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>71</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>70</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E38" s="1">
         <v>1.58</v>
       </c>
-      <c r="F37">
-        <v>1</v>
-      </c>
-      <c r="G37" s="5">
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38" s="5">
         <f t="shared" si="1"/>
         <v>1.58</v>
       </c>
-      <c r="H37" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="2" t="s">
+      <c r="H38" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>75</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>70</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E39" s="1">
         <v>1.05</v>
       </c>
-      <c r="F38">
-        <v>1</v>
-      </c>
-      <c r="G38" s="5">
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39" s="5">
         <f t="shared" si="1"/>
         <v>1.05</v>
       </c>
-      <c r="H38" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="7" t="s">
+      <c r="H39" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+      <c r="B41" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="8">
-        <f>SUM(G3:G38)</f>
-        <v>514.50999999999988</v>
-      </c>
-      <c r="H40" s="8"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
-      <c r="G41" s="9">
-        <f>SUM(H3:H38)</f>
-        <v>32.159999999999997</v>
-      </c>
-      <c r="H41" s="9"/>
+      <c r="G41" s="8">
+        <f>SUM(G3:G39)</f>
+        <v>536.16999999999996</v>
+      </c>
+      <c r="H41" s="8"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
-      <c r="G42" s="10">
-        <f>SUM(G40:H41)</f>
-        <v>546.66999999999985</v>
-      </c>
-      <c r="H42" s="10"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="2"/>
-      <c r="E45" s="1"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="4"/>
+      <c r="G42" s="9">
+        <f>SUM(H3:H39)</f>
+        <v>32.159999999999997</v>
+      </c>
+      <c r="H42" s="9"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="10">
+        <f>SUM(G41:H42)</f>
+        <v>568.32999999999993</v>
+      </c>
+      <c r="H43" s="10"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>
@@ -1622,6 +1640,12 @@
       <c r="E51" s="1"/>
       <c r="G51" s="5"/>
       <c r="H51" s="4"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="2"/>
+      <c r="E52" s="1"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="4"/>
     </row>
   </sheetData>
   <sortState ref="B36:H38">
@@ -1629,13 +1653,13 @@
   </sortState>
   <mergeCells count="9">
     <mergeCell ref="H22:H23"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="B41:F41"/>
     <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A43:F43"/>
     <mergeCell ref="H3:H16"/>
-    <mergeCell ref="G40:H40"/>
     <mergeCell ref="G41:H41"/>
     <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G43:H43"/>
     <mergeCell ref="H18:H19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added receipts, appeased baker...
</commit_message>
<xml_diff>
--- a/reciepts/Casey/Casey Costs.xlsx
+++ b/reciepts/Casey/Casey Costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="87">
   <si>
     <t>P/N</t>
   </si>
@@ -241,9 +241,6 @@
     <t>Spray Paint</t>
   </si>
   <si>
-    <t>Black Paint for Enclosure</t>
-  </si>
-  <si>
     <t>Amber Plexi</t>
   </si>
   <si>
@@ -266,6 +263,18 @@
   </si>
   <si>
     <t>Test wood and cable ties</t>
+  </si>
+  <si>
+    <t>Black Paint for Base</t>
+  </si>
+  <si>
+    <t>Frame mat</t>
+  </si>
+  <si>
+    <t>Frame mat for poster</t>
+  </si>
+  <si>
+    <t>Michael's</t>
   </si>
 </sst>
 </file>
@@ -661,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H52"/>
+  <dimension ref="A2:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44:H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,10 +1235,10 @@
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" t="s">
         <v>76</v>
-      </c>
-      <c r="C26" t="s">
-        <v>77</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
@@ -1289,7 +1298,7 @@
         <v>1</v>
       </c>
       <c r="G28" s="5">
-        <f t="shared" ref="G28:G39" si="1">F28*E28</f>
+        <f t="shared" ref="G28:G40" si="1">F28*E28</f>
         <v>19.63</v>
       </c>
       <c r="H28" s="4">
@@ -1322,10 +1331,10 @@
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" t="s">
         <v>82</v>
-      </c>
-      <c r="C30" t="s">
-        <v>83</v>
       </c>
       <c r="D30" t="s">
         <v>59</v>
@@ -1346,10 +1355,10 @@
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" t="s">
         <v>78</v>
-      </c>
-      <c r="C31" t="s">
-        <v>79</v>
       </c>
       <c r="D31" t="s">
         <v>59</v>
@@ -1370,10 +1379,10 @@
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" t="s">
         <v>80</v>
-      </c>
-      <c r="C32" t="s">
-        <v>81</v>
       </c>
       <c r="D32" t="s">
         <v>59</v>
@@ -1541,7 +1550,7 @@
         <v>74</v>
       </c>
       <c r="C39" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="D39" t="s">
         <v>70</v>
@@ -1560,56 +1569,74 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="7" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" t="s">
+        <v>85</v>
+      </c>
+      <c r="D40" t="s">
+        <v>86</v>
+      </c>
+      <c r="E40" s="1">
+        <v>17.059999999999999</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40" s="5">
+        <f t="shared" si="1"/>
+        <v>17.059999999999999</v>
+      </c>
+      <c r="H40" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
+      <c r="B42" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="8">
-        <f>SUM(G3:G39)</f>
-        <v>536.16999999999996</v>
-      </c>
-      <c r="H41" s="8"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B42" s="7"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
-      <c r="G42" s="9">
-        <f>SUM(H3:H39)</f>
-        <v>32.159999999999997</v>
-      </c>
-      <c r="H42" s="9"/>
+      <c r="G42" s="8">
+        <f>SUM(G3:G40)</f>
+        <v>553.2299999999999</v>
+      </c>
+      <c r="H42" s="8"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
-      <c r="G43" s="10">
-        <f>SUM(G41:H42)</f>
-        <v>568.32999999999993</v>
-      </c>
-      <c r="H43" s="10"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="2"/>
-      <c r="E46" s="1"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="4"/>
+      <c r="G43" s="9">
+        <f>SUM(H3:H40)</f>
+        <v>32.159999999999997</v>
+      </c>
+      <c r="H43" s="9"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="10">
+        <f>SUM(G42:H43)</f>
+        <v>585.38999999999987</v>
+      </c>
+      <c r="H44" s="10"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
@@ -1646,6 +1673,12 @@
       <c r="E52" s="1"/>
       <c r="G52" s="5"/>
       <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="2"/>
+      <c r="E53" s="1"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="4"/>
     </row>
   </sheetData>
   <sortState ref="B36:H38">
@@ -1653,13 +1686,13 @@
   </sortState>
   <mergeCells count="9">
     <mergeCell ref="H22:H23"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="B42:F42"/>
     <mergeCell ref="A43:F43"/>
+    <mergeCell ref="A44:F44"/>
     <mergeCell ref="H3:H16"/>
-    <mergeCell ref="G41:H41"/>
     <mergeCell ref="G42:H42"/>
     <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G44:H44"/>
     <mergeCell ref="H18:H19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>